<commit_message>
Excel data added for the Module options test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CRMUserPipelineData.xlsx
+++ b/src/test/resources/testData/CRMUserPipelineData.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="opportunityCreate" sheetId="1" r:id="rId1"/>
+    <sheet name="modules" sheetId="2" r:id="rId1"/>
+    <sheet name="opportunities" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sale 1</t>
   </si>
@@ -28,6 +29,21 @@
   </si>
   <si>
     <t>Sale 3</t>
+  </si>
+  <si>
+    <t>opportunity</t>
+  </si>
+  <si>
+    <t>module name</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>Calendar</t>
   </si>
 </sst>
 </file>
@@ -76,8 +92,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -86,11 +106,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,22 +444,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2/27 format changes on User CRM Pipeline feature file and step definitions
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CRMUserPipelineData.xlsx
+++ b/src/test/resources/testData/CRMUserPipelineData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="20" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="modules" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sale 1</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Calendar</t>
+  </si>
+  <si>
+    <t>Inventory</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -473,6 +476,11 @@
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel table tests are added and updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CRMUserPipelineData.xlsx
+++ b/src/test/resources/testData/CRMUserPipelineData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="160" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2140" yWindow="160" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="modules" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Sale 1</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>New Sale 3</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -176,12 +182,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -196,6 +205,8 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -621,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -717,34 +728,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>